<commit_message>
Resquests and Responses done
</commit_message>
<xml_diff>
--- a/back-end/Requests.xlsx
+++ b/back-end/Requests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2Semestre\Aplicações na web\aw-project\back-end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6962F3-4859-4DC5-933F-FB4EE93BBAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6118755-93DF-45F6-A845-AC7F677D269A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7339BE56-F3CD-4EA2-BB4E-FEE8F77C3A35}"/>
+    <workbookView xWindow="2940" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{7339BE56-F3CD-4EA2-BB4E-FEE8F77C3A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>BE Service</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>product/meatID</t>
+  </si>
+  <si>
+    <t>user/userID</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,13 +158,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -327,7 +327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,17 +480,17 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +501,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -512,8 +512,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -521,8 +521,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -532,8 +532,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
@@ -543,8 +543,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -552,8 +552,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>3</v>
       </c>
@@ -561,8 +561,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -570,8 +570,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
@@ -581,8 +581,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
@@ -592,8 +592,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
@@ -603,8 +603,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13" t="s">
         <v>12</v>
       </c>
@@ -612,8 +612,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
@@ -623,8 +623,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -632,12 +632,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>